<commit_message>
data: add 2023-05-15 notices
</commit_message>
<xml_diff>
--- a/data/pre_notices/2023-05-13-.xlsx
+++ b/data/pre_notices/2023-05-13-.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,15 +425,432 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>股票名称</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>股票代码</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>公告标题</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>公告日期</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>公告发布时间</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>公告附件</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>九典制药:独立董事关于第三届董事会第十八次会议相关事项的独立意见</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:58:000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642808_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>九典制药:监事会关于2022年限制性股票激励计划第一个归属期激励对象名单的核查意见</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642800_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>九典制药:第三届监事会第十七次会议决议公告</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642766_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>九典制药:关于调整2022年限制性股票激励计划相关事项的公告</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642799_1.pdf?1684172708000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>九典制药:湖南启元律师事务所关于公司2022年限制性股票激励计划相关事项调整、首次授予部分第一个归属期条件成就及部分已授予尚未归属的限制性股票作废事项的法律意见书</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642777_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>九典制药:关于作废部分限制性股票的公告</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642765_1.pdf?1684172801000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>九典制药:关于2022年限制性股票激励计划第一个归属期归属条件成就的公告</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642780_1.pdf?1684172760000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>九典制药:关于延长向不特定对象发行可转换公司债券股东大会决议有效期及授权有效期的公告</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642767_1.pdf?1684174477000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>九典制药:第三届董事会第十八次会议决议公告</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642758_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>九典制药:上海荣正企业咨询服务(集团)股份有限公司关于公司2022年限制性股票激励计划第一个归属期归属条件成就相关事项之独立财务顾问报告</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642761_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>九典制药:关于召开2023年第一次临时股东大会的通知</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642764_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>金牌厨柜</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>603180</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>金牌厨柜:金牌厨柜家居科技股份有限公司2022年年度股东大会会议资料</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:07:41:000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586641321_1.pdf?1684170481000.pdf</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -431,14 +860,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>股票名称</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>股票代码</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>公告数量</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>金牌厨柜</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>603180</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data: add 2023-05-18 notices
</commit_message>
<xml_diff>
--- a/data/pre_notices/2023-05-13-.xlsx
+++ b/data/pre_notices/2023-05-13-.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,81 +468,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金丹科技</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>300829</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>九典制药:独立董事关于第三届董事会第十八次会议相关事项的独立意见</t>
+          <t>金丹科技:关于全资子公司取得营业执照的公告</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-05-16 00:00:00</t>
+          <t>2023-05-17 00:00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:58:000</t>
+          <t>2023-05-17 11:45:48:000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642808_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305171586712182_1.pdf?1684324097000.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金埔园林</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>301098</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>九典制药:监事会关于2022年限制性股票激励计划第一个归属期激励对象名单的核查意见</t>
+          <t>金埔园林:2022年年度权益分派实施公告</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023-05-16 00:00:00</t>
+          <t>2023-05-18 00:00:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-17 17:16:00:000</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642800_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305171586723155_1.pdf?1684343769000.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金埔园林</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>301098</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>九典制药:第三届监事会第十七次会议决议公告</t>
+          <t>金埔园林:江苏世纪同仁律师事务所关于金埔园林股份有限公司2022年年度股东大会的法律意见书</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -552,29 +552,29 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-16 19:08:04:000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642766_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586690253_1.pdf?1684264092000.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金埔园林</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>301098</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>九典制药:关于调整2022年限制性股票激励计划相关事项的公告</t>
+          <t>金埔园林:2022年年度股东大会决议公告</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -584,29 +584,29 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-16 19:07:44:000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642799_1.pdf?1684172708000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586690224_1.pdf?1684267535000.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金埔园林</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>301098</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>九典制药:湖南启元律师事务所关于公司2022年限制性股票激励计划相关事项调整、首次授予部分第一个归属期条件成就及部分已授予尚未归属的限制性股票作废事项的法律意见书</t>
+          <t>金埔园林:关于对外担保的进展公告</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -616,29 +616,29 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-16 19:07:44:000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642777_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586690223_1.pdf?1684264084000.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金埔园林</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>301098</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>九典制药:关于作废部分限制性股票的公告</t>
+          <t>金埔园林:关于与兰坪白族普米族自治县人民政府签订战略合作框架协议的公告</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -648,12 +648,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-16 19:05:59:000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642765_1.pdf?1684172801000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586689989_1.pdf?1684263959000.pdf</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>九典制药:关于2022年限制性股票激励计划第一个归属期归属条件成就的公告</t>
+          <t>九典制药:300705九典制药调研活动信息20230516</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -680,12 +680,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-16 17:24:32:000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642780_1.pdf?1684172760000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586686122_1.pdf?1684257884000.pdf</t>
         </is>
       </c>
     </row>
@@ -702,7 +702,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>九典制药:关于延长向不特定对象发行可转换公司债券股东大会决议有效期及授权有效期的公告</t>
+          <t>九典制药:独立董事关于第三届董事会第十八次会议相关事项的独立意见</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -712,12 +712,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-05-15 17:40:54:000</t>
+          <t>2023-05-15 17:40:58:000</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642767_1.pdf?1684174477000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642808_1.pdf?1684172462000.pdf</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>九典制药:第三届董事会第十八次会议决议公告</t>
+          <t>九典制药:监事会关于2022年限制性股票激励计划第一个归属期激励对象名单的核查意见</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642758_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642800_1.pdf?1684225278000.pdf</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>九典制药:上海荣正企业咨询服务(集团)股份有限公司关于公司2022年限制性股票激励计划第一个归属期归属条件成就相关事项之独立财务顾问报告</t>
+          <t>九典制药:第三届监事会第十七次会议决议公告</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642761_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642766_1.pdf?1684225564000.pdf</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>九典制药:关于召开2023年第一次临时股东大会的通知</t>
+          <t>九典制药:关于调整2022年限制性股票激励计划相关事项的公告</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -813,39 +813,551 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642764_1.pdf?1684172462000.pdf</t>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642799_1.pdf?1684172708000.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>九典制药:湖南启元律师事务所关于公司2022年限制性股票激励计划相关事项调整、首次授予部分第一个归属期条件成就及部分已授予尚未归属的限制性股票作废事项的法律意见书</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642777_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>九典制药:关于作废部分限制性股票的公告</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642765_1.pdf?1684172801000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>九典制药:关于2022年限制性股票激励计划第一个归属期归属条件成就的公告</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642780_1.pdf?1684172760000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>九典制药:关于延长向不特定对象发行可转换公司债券股东大会决议有效期及授权有效期的公告</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642767_1.pdf?1684174477000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>九典制药:第三届董事会第十八次会议决议公告</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642758_1.pdf?1684235003000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>九典制药:上海荣正企业咨询服务(集团)股份有限公司关于公司2022年限制性股票激励计划第一个归属期归属条件成就相关事项之独立财务顾问报告</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642761_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>九典制药:关于召开2023年第一次临时股东大会的通知</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-05-15 17:40:54:000</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586642764_1.pdf?1684172462000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>佳禾智能</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>300793</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>佳禾智能:2022年度股东大会法律意见书</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2023-05-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-05-18 18:34:00:000</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305181586762915_1.pdf?1684434840000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>佳禾智能</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>300793</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>佳禾智能:2022年度股东大会决议公告</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2023-05-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2023-05-18 18:34:00:000</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305181586762911_1.pdf?1684434840000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>佳禾智能</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>300793</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>佳禾智能:300793佳禾智能调研活动信息20230516</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-05-16 19:10:39:000</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586690280_1.pdf?1684264256000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>金牌厨柜</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>603180</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>金牌厨柜:金牌厨柜关于2022年度业绩说明会召开情况的公告</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2023-05-17 00:00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2023-05-16 17:22:52:000</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586686132_1.pdf?1684257887000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>金牌厨柜</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>603180</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>金牌厨柜:金牌厨柜关于签订募集资金专户存储四方监管协议公告</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2023-05-17 00:00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2023-05-16 17:22:52:000</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305161586686141_1.pdf?1684310250000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>金牌厨柜</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>603180</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>金牌厨柜:金牌厨柜家居科技股份有限公司2022年年度股东大会会议资料</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2023-05-16 00:00:00</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2023-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>2023-05-15 17:07:41:000</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305151586641321_1.pdf?1684170481000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>星帅尔</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>002860</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>星帅尔:关于2022年限制性股票激励计划预留部分限制性股票登记完成的公告</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2023-05-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2023-05-18 19:54:05:000</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305181586835614_1.pdf?1684439649000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>星帅尔</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>002860</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>星帅尔:关于公司取得专利证书的公告</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2023-05-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2023-05-18 18:02:55:000</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305181586760878_1.pdf?1684432991000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>星帅尔</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>002860</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>星帅尔:锦天城关于星帅尔2022年年度股东大会的法律意见书</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2023-05-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2023-05-18 18:02:26:000</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305181586760849_1.pdf?1684432979000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>星帅尔</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>002860</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>星帅尔:2022年年度股东大会决议公告</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2023-05-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2023-05-18 18:00:02:000</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305181586758798_1.pdf?1684432810000.pdf</t>
         </is>
       </c>
     </row>
@@ -860,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -888,31 +1400,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>九典制药</t>
+          <t>金丹科技</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>300705</t>
+          <t>300829</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>金埔园林</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>301098</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>九典制药</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>300705</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>佳禾智能</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>300793</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>金牌厨柜</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>603180</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>星帅尔</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>002860</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>